<commit_message>
Correção doc modelo de evid. de testes + 1os testes do card MHS-15
</commit_message>
<xml_diff>
--- a/Testes/Documento de Testes - MHS - MODELO.xlsx
+++ b/Testes/Documento de Testes - MHS - MODELO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Meus Projetos\My Hair Salon\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F435214B-1E6B-484D-8AD7-B91A0F946273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012EA85-F84E-479A-B54C-DE48D117F41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{60EB7970-8BE6-4BE5-9238-E82C81D98BC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Informações Gerais" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -199,8 +199,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A0962-7C6C-4640-A9C3-D61D95AF0094}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -706,7 +709,7 @@
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -714,7 +717,7 @@
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -722,7 +725,7 @@
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -730,7 +733,7 @@
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -738,7 +741,7 @@
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -746,7 +749,7 @@
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -754,7 +757,7 @@
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -779,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8ABBC-E64F-4728-8C3E-82E71C484C73}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,92 +852,92 @@
     </row>
     <row r="7" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="6"/>
     </row>
   </sheetData>

</xml_diff>